<commit_message>
Item matches as list
</commit_message>
<xml_diff>
--- a/Files/Catcher.xlsx
+++ b/Files/Catcher.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="72">
   <si>
     <t>Hora</t>
   </si>
@@ -254,6 +254,18 @@
   </si>
   <si>
     <t>10:58</t>
+  </si>
+  <si>
+    <t>11:28</t>
+  </si>
+  <si>
+    <t>15:19</t>
+  </si>
+  <si>
+    <t>16:45</t>
+  </si>
+  <si>
+    <t>21:28</t>
   </si>
 </sst>
 </file>
@@ -3230,7 +3242,7 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3278,6 +3290,62 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3285,7 +3353,7 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3333,6 +3401,62 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3340,7 +3464,7 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3388,6 +3512,62 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3395,7 +3575,7 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3441,6 +3621,62 @@
       </c>
       <c r="D3">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Category matching split as list
</commit_message>
<xml_diff>
--- a/Files/Catcher.xlsx
+++ b/Files/Catcher.xlsx
@@ -44,13 +44,17 @@
     <sheet name="22 - 9 Mango" sheetId="35" r:id="rId35"/>
     <sheet name="22 - 9 Zara" sheetId="36" r:id="rId36"/>
     <sheet name="22 - 9 Stradivarius" sheetId="37" r:id="rId37"/>
+    <sheet name="23 - 9 Mango" sheetId="38" r:id="rId38"/>
+    <sheet name="23 - 9 Zara" sheetId="39" r:id="rId39"/>
+    <sheet name="23 - 9 Stradivarius" sheetId="40" r:id="rId40"/>
+    <sheet name="23 - 9 Bershka" sheetId="41" r:id="rId41"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="72">
   <si>
     <t>Hora</t>
   </si>
@@ -3684,6 +3688,60 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D10"/>
@@ -3837,6 +3895,60 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>

</xml_diff>

<commit_message>
Pull & Bear crawling
</commit_message>
<xml_diff>
--- a/Files/Catcher.xlsx
+++ b/Files/Catcher.xlsx
@@ -56,13 +56,18 @@
     <sheet name="27 - 9 Zara" sheetId="47" r:id="rId47"/>
     <sheet name="27 - 9 Stradivarius" sheetId="48" r:id="rId48"/>
     <sheet name="27 - 9 Bershka" sheetId="49" r:id="rId49"/>
+    <sheet name="29 - 9 PullAndBear" sheetId="50" r:id="rId50"/>
+    <sheet name="29 - 9 Mango" sheetId="51" r:id="rId51"/>
+    <sheet name="29 - 9 Zara" sheetId="52" r:id="rId52"/>
+    <sheet name="29 - 9 Stradivarius" sheetId="53" r:id="rId53"/>
+    <sheet name="29 - 9 Bershka" sheetId="54" r:id="rId54"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="90">
   <si>
     <t>Hora</t>
   </si>
@@ -299,6 +304,39 @@
   </si>
   <si>
     <t>20:37</t>
+  </si>
+  <si>
+    <t>17:13</t>
+  </si>
+  <si>
+    <t>17:41</t>
+  </si>
+  <si>
+    <t>17:52</t>
+  </si>
+  <si>
+    <t>17:53</t>
+  </si>
+  <si>
+    <t>17:55</t>
+  </si>
+  <si>
+    <t>17:56</t>
+  </si>
+  <si>
+    <t>18:8</t>
+  </si>
+  <si>
+    <t>18:24</t>
+  </si>
+  <si>
+    <t>18:27</t>
+  </si>
+  <si>
+    <t>20:1</t>
+  </si>
+  <si>
+    <t>20:8</t>
   </si>
 </sst>
 </file>
@@ -4627,6 +4665,981 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>

</xml_diff>

<commit_message>
No-stock checks on database
</commit_message>
<xml_diff>
--- a/Files/Catcher.xlsx
+++ b/Files/Catcher.xlsx
@@ -71,13 +71,18 @@
     <sheet name="1 - 10 Zara" sheetId="62" r:id="rId62"/>
     <sheet name="1 - 10 Stradivarius" sheetId="63" r:id="rId63"/>
     <sheet name="1 - 10 Bershka" sheetId="64" r:id="rId64"/>
+    <sheet name="5 - 10 PullAndBear" sheetId="65" r:id="rId65"/>
+    <sheet name="5 - 10 Mango" sheetId="66" r:id="rId66"/>
+    <sheet name="5 - 10 Zara" sheetId="67" r:id="rId67"/>
+    <sheet name="5 - 10 Stradivarius" sheetId="68" r:id="rId68"/>
+    <sheet name="5 - 10 Bershka" sheetId="69" r:id="rId69"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="117">
   <si>
     <t>Hora</t>
   </si>
@@ -422,6 +427,12 @@
   </si>
   <si>
     <t>1:51</t>
+  </si>
+  <si>
+    <t>23:6</t>
+  </si>
+  <si>
+    <t>23:7</t>
   </si>
 </sst>
 </file>
@@ -7856,6 +7867,211 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>

</xml_diff>

<commit_message>
Bags and Accessories subcategories added
</commit_message>
<xml_diff>
--- a/Files/Catcher.xlsx
+++ b/Files/Catcher.xlsx
@@ -76,13 +76,18 @@
     <sheet name="5 - 10 Zara" sheetId="67" r:id="rId67"/>
     <sheet name="5 - 10 Stradivarius" sheetId="68" r:id="rId68"/>
     <sheet name="5 - 10 Bershka" sheetId="69" r:id="rId69"/>
+    <sheet name="6 - 10 PullAndBear" sheetId="70" r:id="rId70"/>
+    <sheet name="6 - 10 Mango" sheetId="71" r:id="rId71"/>
+    <sheet name="6 - 10 Zara" sheetId="72" r:id="rId72"/>
+    <sheet name="6 - 10 Stradivarius" sheetId="73" r:id="rId73"/>
+    <sheet name="6 - 10 Bershka" sheetId="74" r:id="rId74"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="117">
   <si>
     <t>Hora</t>
   </si>
@@ -8155,6 +8160,141 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>

</xml_diff>

<commit_message>
Speed modification to Crawler proccess
</commit_message>
<xml_diff>
--- a/Files/Catcher.xlsx
+++ b/Files/Catcher.xlsx
@@ -104,13 +104,25 @@
     <sheet name="11 - 10 Stradivarius" sheetId="95" r:id="rId95"/>
     <sheet name="11 - 10 Bershka" sheetId="96" r:id="rId96"/>
     <sheet name="11 - 10 MercedesCampuzano" sheetId="97" r:id="rId97"/>
+    <sheet name="12 - 10 PullAndBear" sheetId="98" r:id="rId98"/>
+    <sheet name="12 - 10 Mango" sheetId="99" r:id="rId99"/>
+    <sheet name="12 - 10 Zara" sheetId="100" r:id="rId100"/>
+    <sheet name="12 - 10 Stradivarius" sheetId="101" r:id="rId101"/>
+    <sheet name="12 - 10 Bershka" sheetId="102" r:id="rId102"/>
+    <sheet name="12 - 10 MercedesCampuzano" sheetId="103" r:id="rId103"/>
+    <sheet name="13 - 10 MercedesCampuzano" sheetId="104" r:id="rId104"/>
+    <sheet name="13 - 10 PullAndBear" sheetId="105" r:id="rId105"/>
+    <sheet name="13 - 10 Mango" sheetId="106" r:id="rId106"/>
+    <sheet name="13 - 10 Zara" sheetId="107" r:id="rId107"/>
+    <sheet name="13 - 10 Stradivarius" sheetId="108" r:id="rId108"/>
+    <sheet name="13 - 10 Bershka" sheetId="109" r:id="rId109"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="131">
   <si>
     <t>Hora</t>
   </si>
@@ -481,7 +493,28 @@
     <t>9:36</t>
   </si>
   <si>
+    <t>21:1</t>
+  </si>
+  <si>
     <t>9:40</t>
+  </si>
+  <si>
+    <t>21:2</t>
+  </si>
+  <si>
+    <t>22:9</t>
+  </si>
+  <si>
+    <t>21:36</t>
+  </si>
+  <si>
+    <t>23:28</t>
+  </si>
+  <si>
+    <t>23:31</t>
+  </si>
+  <si>
+    <t>0:6</t>
   </si>
 </sst>
 </file>
@@ -1059,6 +1092,430 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet100.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet101.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet102.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet103.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet104.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet105.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet106.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet107.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet108.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet109.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D8"/>
@@ -9078,7 +9535,7 @@
 
 <file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9196,6 +9653,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9203,7 +9674,7 @@
 
 <file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9309,7 +9780,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
@@ -9335,6 +9806,90 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9342,7 +9897,7 @@
 
 <file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9448,7 +10003,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
@@ -9474,6 +10029,90 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9481,7 +10120,7 @@
 
 <file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9587,7 +10226,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
@@ -9613,6 +10252,90 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9620,7 +10343,7 @@
 
 <file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9726,7 +10449,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
@@ -9752,6 +10475,90 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9782,4 +10589,114 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet99.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>